<commit_message>
GPLIM-4712 fixes and refactoring. Passes dbFree tests
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\mercury\mercury\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25200" yWindow="-7245" windowWidth="25200" windowHeight="19665"/>
+    <workbookView xWindow="1400" yWindow="1180" windowWidth="27880" windowHeight="10760"/>
   </bookViews>
   <sheets>
     <sheet name="New Technology Lib Kit" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="109">
   <si>
     <t>Total Library Volume (ul)</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -342,6 +337,21 @@
   </si>
   <si>
     <t>AAGGCTAT</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>enz1</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>One</t>
   </si>
 </sst>
 </file>
@@ -351,7 +361,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -965,7 +975,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="150">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -1119,6 +1129,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1232,7 +1247,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="150">
+  <cellStyles count="155">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="120"/>
     <cellStyle name="20% - Accent2" xfId="93" builtinId="34" customBuiltin="1"/>
@@ -1350,6 +1365,11 @@
     <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="77" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="73" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="74" builtinId="17" customBuiltin="1"/>
@@ -1778,56 +1798,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:AN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W16" workbookViewId="0">
-      <selection activeCell="Y31" sqref="Y31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="41" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="41" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39" style="41" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="41" customWidth="1"/>
-    <col min="8" max="8" width="38.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.42578125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" style="7" customWidth="1"/>
-    <col min="13" max="13" width="46.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.42578125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="48.28515625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="29.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.42578125" style="7" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="20.42578125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="7" customWidth="1"/>
-    <col min="23" max="23" width="25.28515625" style="7" customWidth="1"/>
-    <col min="24" max="24" width="8.7109375" style="7" customWidth="1"/>
-    <col min="25" max="25" width="40.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="46.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="25.140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="41" customWidth="1"/>
+    <col min="8" max="8" width="38.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.5" style="7" customWidth="1"/>
+    <col min="11" max="11" width="26.5" style="7" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="46.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.5" style="7" customWidth="1"/>
+    <col min="15" max="15" width="48.33203125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="29.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.5" style="7" customWidth="1"/>
+    <col min="18" max="18" width="15.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="20.5" style="7" customWidth="1"/>
+    <col min="22" max="22" width="9.5" style="7" customWidth="1"/>
+    <col min="23" max="23" width="25.33203125" style="7" customWidth="1"/>
+    <col min="24" max="24" width="8.6640625" style="7" customWidth="1"/>
+    <col min="25" max="25" width="40.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="46.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.1640625" style="7" customWidth="1"/>
     <col min="31" max="31" width="31" style="7" customWidth="1"/>
-    <col min="32" max="32" width="25.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="48.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="48.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="8" style="7" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="20.42578125" style="7"/>
+    <col min="42" max="16384" width="20.5" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17">
@@ -2156,17 +2176,17 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="25.5">
+    <row r="23" spans="1:40" ht="24">
       <c r="B23" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="38.25">
+    <row r="24" spans="1:40" ht="24">
       <c r="B24" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="25.5">
+    <row r="25" spans="1:40" ht="24">
       <c r="B25" s="26" t="s">
         <v>25</v>
       </c>
@@ -2236,7 +2256,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:40" s="29" customFormat="1" ht="76.5">
+    <row r="29" spans="1:40" s="29" customFormat="1" ht="60">
       <c r="A29" s="30" t="s">
         <v>3</v>
       </c>
@@ -2377,7 +2397,18 @@
       <c r="F30" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="G30" s="46"/>
+      <c r="G30" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="H30" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="J30" s="47" t="s">
+        <v>104</v>
+      </c>
       <c r="K30" s="45" t="s">
         <v>80</v>
       </c>
@@ -2396,15 +2427,30 @@
       <c r="P30" s="47" t="s">
         <v>85</v>
       </c>
+      <c r="Q30" s="47">
+        <v>12345</v>
+      </c>
       <c r="R30" s="45">
         <v>293</v>
       </c>
       <c r="S30" s="45">
         <v>419</v>
       </c>
+      <c r="T30" s="47">
+        <v>123</v>
+      </c>
       <c r="U30" s="45" t="s">
         <v>73</v>
       </c>
+      <c r="V30" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="W30" s="47">
+        <v>123456789</v>
+      </c>
+      <c r="X30" s="47" t="s">
+        <v>107</v>
+      </c>
       <c r="Y30" s="45" t="s">
         <v>103</v>
       </c>
@@ -2431,6 +2477,9 @@
       </c>
       <c r="AG30" s="47" t="s">
         <v>87</v>
+      </c>
+      <c r="AH30" s="47" t="s">
+        <v>108</v>
       </c>
       <c r="AI30" s="45" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
GPLIM-4712 unit test fixes
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1180" windowWidth="27880" windowHeight="10760"/>
+    <workbookView xWindow="40" yWindow="20" windowWidth="28000" windowHeight="6740"/>
   </bookViews>
   <sheets>
     <sheet name="New Technology Lib Kit" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
   <si>
     <t>Total Library Volume (ul)</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -237,9 +237,6 @@
     <t>SQUID Project</t>
   </si>
   <si>
-    <t>Illumina</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>Nextera</t>
   </si>
   <si>
-    <t>0098972718</t>
-  </si>
-  <si>
     <t>Poon - LLDeep samples for Low-Input Metagenomic</t>
   </si>
   <si>
@@ -264,9 +258,6 @@
     <t>MOCK1</t>
   </si>
   <si>
-    <t>SM-AYA5T</t>
-  </si>
-  <si>
     <t>MOCK.FSK1.A</t>
   </si>
   <si>
@@ -288,9 +279,6 @@
     <t>GPE8X</t>
   </si>
   <si>
-    <t>1 lane HiSeq 2500</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -352,6 +340,15 @@
   </si>
   <si>
     <t>One</t>
+  </si>
+  <si>
+    <t>E0098972718</t>
+  </si>
+  <si>
+    <t>Lib-MOCK.FSK1.A</t>
+  </si>
+  <si>
+    <t>NovaSeq</t>
   </si>
 </sst>
 </file>
@@ -975,7 +972,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -1134,6 +1131,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1247,7 +1245,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="156">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="120"/>
     <cellStyle name="20% - Accent2" xfId="93" builtinId="34" customBuiltin="1"/>
@@ -1370,6 +1368,7 @@
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="77" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="73" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="74" builtinId="17" customBuiltin="1"/>
@@ -1801,10 +1800,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AN30"/>
+  <dimension ref="A2:AL30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="AM24" sqref="AM1:AN1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1844,10 +1843,8 @@
     <col min="36" max="36" width="24.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="20.5" style="7"/>
+    <col min="39" max="39" width="13" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="20.5" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17">
@@ -1888,7 +1885,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
@@ -1908,7 +1905,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -1927,7 +1924,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
@@ -1947,7 +1944,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
@@ -1983,7 +1980,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
@@ -2002,7 +1999,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
@@ -2038,7 +2035,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
@@ -2056,7 +2053,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -2074,7 +2071,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F14" s="40"/>
       <c r="G14" s="40"/>
@@ -2105,7 +2102,7 @@
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:38">
       <c r="B17" s="19" t="s">
         <v>41</v>
       </c>
@@ -2120,7 +2117,7 @@
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:38">
       <c r="B18" s="19" t="s">
         <v>44</v>
       </c>
@@ -2135,12 +2132,12 @@
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:38">
       <c r="B19" s="19" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
@@ -2151,12 +2148,12 @@
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:38">
       <c r="B20" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F20" s="37"/>
       <c r="G20" s="37"/>
@@ -2168,36 +2165,36 @@
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:38">
       <c r="B22" s="19" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:40" ht="24">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" ht="24">
       <c r="B23" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="24">
+    <row r="24" spans="1:38" ht="24">
       <c r="B24" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="24">
+    <row r="25" spans="1:38" ht="24">
       <c r="B25" s="26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:38">
       <c r="B26" s="19"/>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:38">
       <c r="B27" s="19"/>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:38">
       <c r="A28" s="27" t="s">
         <v>8</v>
       </c>
@@ -2256,7 +2253,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:40" s="29" customFormat="1" ht="60">
+    <row r="29" spans="1:38" s="29" customFormat="1" ht="60">
       <c r="A29" s="30" t="s">
         <v>3</v>
       </c>
@@ -2371,61 +2368,55 @@
       <c r="AL29" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AM29" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN29" s="43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:40" s="47" customFormat="1">
+    </row>
+    <row r="30" spans="1:38" s="47" customFormat="1">
       <c r="A30" s="45">
         <v>22</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D30" s="46">
         <v>963357</v>
       </c>
       <c r="E30" s="47" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F30" s="45" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="G30" s="46" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H30" s="47" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I30" s="47" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J30" s="47" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K30" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="L30" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="M30" t="s">
+        <v>106</v>
+      </c>
+      <c r="N30" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="L30" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="M30" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="N30" s="47" t="s">
-        <v>83</v>
-      </c>
       <c r="O30" s="47" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P30" s="47" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Q30" s="47">
         <v>12345</v>
@@ -2440,22 +2431,22 @@
         <v>123</v>
       </c>
       <c r="U30" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V30" s="47" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="W30" s="47">
         <v>123456789</v>
       </c>
       <c r="X30" s="47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Y30" s="45" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Z30" s="45" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="AA30" s="45">
         <v>96</v>
@@ -2464,40 +2455,34 @@
         <v>7.4000000953674316</v>
       </c>
       <c r="AC30" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD30" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE30" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF30" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG30" s="47">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI30" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="AD30" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE30" s="45" t="s">
+      <c r="AJ30" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK30" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL30" s="45" t="s">
         <v>75</v>
-      </c>
-      <c r="AF30" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG30" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH30" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI30" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ30" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK30" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="AL30" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM30" s="46">
-        <v>963357</v>
-      </c>
-      <c r="AN30" s="47" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPLIM-4712 Add barcode update spreadsheet
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
   <si>
     <t>Total Library Volume (ul)</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -349,6 +349,18 @@
   </si>
   <si>
     <t>NovaSeq</t>
+  </si>
+  <si>
+    <t>MOCK.FSK1.B</t>
+  </si>
+  <si>
+    <t>MOCK.FSK1.C</t>
+  </si>
+  <si>
+    <t>Lib-MOCK.FSK1.B</t>
+  </si>
+  <si>
+    <t>Lib-MOCK.FSK1.C</t>
   </si>
 </sst>
 </file>
@@ -972,7 +984,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="156">
+  <cellStyleXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -1132,6 +1144,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1245,7 +1261,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="156">
+  <cellStyles count="160">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="120"/>
     <cellStyle name="20% - Accent2" xfId="93" builtinId="34" customBuiltin="1"/>
@@ -1369,6 +1385,10 @@
     <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="77" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="73" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="74" builtinId="17" customBuiltin="1"/>
@@ -1800,10 +1820,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AL30"/>
+  <dimension ref="A2:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="AM24" sqref="AM1:AN1048576"/>
+    <sheetView tabSelected="1" topLeftCell="P28" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2485,6 +2505,174 @@
         <v>75</v>
       </c>
     </row>
+    <row r="31" spans="1:38" s="47" customFormat="1">
+      <c r="A31" s="7"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="L31" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="M31" t="s">
+        <v>110</v>
+      </c>
+      <c r="N31" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="O31" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="P31" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="45">
+        <v>293</v>
+      </c>
+      <c r="S31" s="45">
+        <v>419</v>
+      </c>
+      <c r="T31" s="22"/>
+      <c r="U31" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="V31" s="22"/>
+      <c r="W31" s="22"/>
+      <c r="X31" s="22"/>
+      <c r="Y31" s="22"/>
+      <c r="Z31" s="22"/>
+      <c r="AA31" s="45">
+        <v>97</v>
+      </c>
+      <c r="AB31" s="45">
+        <v>8</v>
+      </c>
+      <c r="AC31" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD31" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE31" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF31" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG31" s="47">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI31" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ31" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK31" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL31" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" s="47" customFormat="1">
+      <c r="A32" s="7"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="L32" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="M32" t="s">
+        <v>111</v>
+      </c>
+      <c r="N32" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="O32" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="P32" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="45">
+        <v>293</v>
+      </c>
+      <c r="S32" s="45">
+        <v>419</v>
+      </c>
+      <c r="T32" s="22"/>
+      <c r="U32" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="22"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="22"/>
+      <c r="AA32" s="45">
+        <v>98</v>
+      </c>
+      <c r="AB32" s="45">
+        <v>9</v>
+      </c>
+      <c r="AC32" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD32" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE32" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF32" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG32" s="47">
+        <v>1</v>
+      </c>
+      <c r="AH32" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI32" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ32" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK32" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL32" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="M6:N6"/>

</xml_diff>

<commit_message>
GPLIM-4712 external library spreadsheet aggregation particle and analysis type fixes, and other fixes
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="20" windowWidth="28000" windowHeight="6740"/>
+    <workbookView xWindow="60" yWindow="20" windowWidth="28000" windowHeight="6740"/>
   </bookViews>
   <sheets>
     <sheet name="New Technology Lib Kit" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
   <si>
     <t>Total Library Volume (ul)</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -270,12 +270,6 @@
     <t>WholeGenomeShotgun</t>
   </si>
   <si>
-    <t>WholeGenomeShotgunwithoutReference</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>GPE8X</t>
   </si>
   <si>
@@ -361,6 +355,15 @@
   </si>
   <si>
     <t>Lib-MOCK.FSK1.C</t>
+  </si>
+  <si>
+    <t>WholeGenomeShotgun.AssemblyWithoutReference</t>
+  </si>
+  <si>
+    <t>Homo_sapiens_RP11-78M2</t>
+  </si>
+  <si>
+    <t>Homo_sapiens_RP11-78M2|-1</t>
   </si>
 </sst>
 </file>
@@ -984,7 +987,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="160">
+  <cellStyleXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -1148,6 +1151,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1261,7 +1268,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="160">
+  <cellStyles count="164">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="120"/>
     <cellStyle name="20% - Accent2" xfId="93" builtinId="34" customBuiltin="1"/>
@@ -1389,6 +1396,10 @@
     <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="77" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="73" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="74" builtinId="17" customBuiltin="1"/>
@@ -1822,8 +1833,8 @@
   </sheetPr>
   <dimension ref="A2:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P28" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="J28" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1905,7 +1916,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
@@ -1925,7 +1936,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -1944,7 +1955,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
@@ -1964,7 +1975,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
@@ -2000,7 +2011,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
@@ -2019,7 +2030,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
@@ -2055,7 +2066,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
@@ -2073,7 +2084,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -2091,7 +2102,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F14" s="40"/>
       <c r="G14" s="40"/>
@@ -2157,7 +2168,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
@@ -2173,7 +2184,7 @@
         <v>43</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F20" s="37"/>
       <c r="G20" s="37"/>
@@ -2190,7 +2201,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:38" ht="24">
@@ -2394,7 +2405,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C30" s="46" t="s">
         <v>79</v>
@@ -2403,22 +2414,22 @@
         <v>963357</v>
       </c>
       <c r="E30" s="47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F30" s="45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G30" s="46" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H30" s="47" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I30" s="47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J30" s="47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K30" s="45" t="s">
         <v>77</v>
@@ -2427,16 +2438,16 @@
         <v>76</v>
       </c>
       <c r="M30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N30" s="47" t="s">
         <v>80</v>
       </c>
       <c r="O30" s="47" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="P30" s="47" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="Q30" s="47">
         <v>12345</v>
@@ -2454,16 +2465,16 @@
         <v>72</v>
       </c>
       <c r="V30" s="47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="W30" s="47">
         <v>123456789</v>
       </c>
       <c r="X30" s="47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Y30" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Z30" s="45" t="s">
         <v>78</v>
@@ -2484,22 +2495,22 @@
         <v>73</v>
       </c>
       <c r="AF30" s="48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AG30" s="47">
         <v>1</v>
       </c>
       <c r="AH30" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI30" s="45" t="s">
         <v>71</v>
       </c>
       <c r="AJ30" s="47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AK30" s="47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AL30" s="45" t="s">
         <v>75</v>
@@ -2512,29 +2523,29 @@
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
       <c r="F31" s="45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
       <c r="J31" s="22"/>
       <c r="K31" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L31" s="45" t="s">
         <v>76</v>
       </c>
       <c r="M31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N31" s="47" t="s">
         <v>80</v>
       </c>
       <c r="O31" s="47" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="P31" s="47" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="Q31" s="22"/>
       <c r="R31" s="45">
@@ -2568,22 +2579,22 @@
         <v>73</v>
       </c>
       <c r="AF31" s="48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AG31" s="47">
         <v>1</v>
       </c>
       <c r="AH31" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI31" s="45" t="s">
         <v>71</v>
       </c>
       <c r="AJ31" s="47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AK31" s="47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AL31" s="45" t="s">
         <v>75</v>
@@ -2596,29 +2607,29 @@
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
       <c r="F32" s="45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
       <c r="K32" s="45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L32" s="45" t="s">
         <v>76</v>
       </c>
       <c r="M32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N32" s="47" t="s">
         <v>80</v>
       </c>
       <c r="O32" s="47" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="P32" s="47" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="Q32" s="22"/>
       <c r="R32" s="45">
@@ -2652,22 +2663,22 @@
         <v>73</v>
       </c>
       <c r="AF32" s="48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AG32" s="47">
         <v>1</v>
       </c>
       <c r="AH32" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI32" s="45" t="s">
         <v>71</v>
       </c>
       <c r="AJ32" s="47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AK32" s="47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AL32" s="45" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
GPLIM-4712_AggParticle fix EZPass, all tests pass
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="20" windowWidth="28000" windowHeight="6740"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
   </bookViews>
   <sheets>
     <sheet name="New Technology Lib Kit" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="125">
   <si>
     <t>Total Library Volume (ul)</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -246,12 +246,6 @@
     <t>Nextera</t>
   </si>
   <si>
-    <t>Poon - LLDeep samples for Low-Input Metagenomic</t>
-  </si>
-  <si>
-    <t>SSF-1344</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -276,9 +270,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>Tiffany Poon</t>
-  </si>
-  <si>
     <t>G96214</t>
   </si>
   <si>
@@ -364,15 +355,57 @@
   </si>
   <si>
     <t>Homo_sapiens_RP11-78M2|-1</t>
+  </si>
+  <si>
+    <t>E0098972719</t>
+  </si>
+  <si>
+    <t>E0098972720</t>
+  </si>
+  <si>
+    <t>917994.1</t>
+  </si>
+  <si>
+    <t>917994.2</t>
+  </si>
+  <si>
+    <t>G96215</t>
+  </si>
+  <si>
+    <t>963357.0</t>
+  </si>
+  <si>
+    <t>Poon - Low Input Metagenomic_CMIT</t>
+  </si>
+  <si>
+    <t>Poon - Low Input Nextera_SSF-1648_ACE/Prism</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>MOCK2</t>
+  </si>
+  <si>
+    <t>sample info 1</t>
+  </si>
+  <si>
+    <t>analysis info 1</t>
+  </si>
+  <si>
+    <t>asi4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   aaai4</t>
+  </si>
+  <si>
+    <t>Lib-MOCK.FSK1.A2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -614,7 +647,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,12 +866,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -987,7 +1014,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="164">
+  <cellStyleXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -1155,8 +1182,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1169,19 +1214,11 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1190,85 +1227,64 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="8" fillId="40" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="164">
+  <cellStyles count="182">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="120"/>
     <cellStyle name="20% - Accent2" xfId="93" builtinId="34" customBuiltin="1"/>
@@ -1400,6 +1416,24 @@
     <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="77" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="73" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="74" builtinId="17" customBuiltin="1"/>
@@ -1831,857 +1865,939 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AL32"/>
+  <dimension ref="A2:AL33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J28" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="41" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39" style="41" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="41" customWidth="1"/>
-    <col min="8" max="8" width="38.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.5" style="7" customWidth="1"/>
-    <col min="11" max="11" width="26.5" style="7" customWidth="1"/>
-    <col min="12" max="12" width="28.83203125" style="7" customWidth="1"/>
-    <col min="13" max="13" width="46.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.5" style="7" customWidth="1"/>
-    <col min="15" max="15" width="48.33203125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="29.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.5" style="7" customWidth="1"/>
-    <col min="18" max="18" width="15.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="20.5" style="7" customWidth="1"/>
-    <col min="22" max="22" width="9.5" style="7" customWidth="1"/>
-    <col min="23" max="23" width="25.33203125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="8.6640625" style="7" customWidth="1"/>
-    <col min="25" max="25" width="40.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="46.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="25.1640625" style="7" customWidth="1"/>
-    <col min="31" max="31" width="31" style="7" customWidth="1"/>
-    <col min="32" max="32" width="25.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="48.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="20.5" style="7"/>
+    <col min="1" max="1" width="15.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="38.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="26.5" style="3" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="46.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.5" style="3" customWidth="1"/>
+    <col min="15" max="15" width="48.33203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="29.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.5" style="3" customWidth="1"/>
+    <col min="18" max="18" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="20.5" style="3" customWidth="1"/>
+    <col min="22" max="22" width="9.5" style="3" customWidth="1"/>
+    <col min="23" max="23" width="25.33203125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="8.6640625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="40.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="46.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.1640625" style="3" customWidth="1"/>
+    <col min="31" max="31" width="31" style="3" customWidth="1"/>
+    <col min="32" max="32" width="25.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="48.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="20.5" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17">
       <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="C2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
       <c r="M2" s="4"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="2:17">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="3"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-    </row>
-    <row r="5" spans="2:17">
-      <c r="B5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="38" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="3"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-    </row>
-    <row r="6" spans="2:17">
-      <c r="B6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="38" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-    </row>
-    <row r="7" spans="2:17">
-      <c r="B7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="38" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2215</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="10"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="2:17">
-      <c r="B8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="3"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="2:17">
-      <c r="B9" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="37" t="s">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="2:17">
-      <c r="B10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="37" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="20"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="2:17">
-      <c r="B11" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="37">
-        <v>2215</v>
-      </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="20"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="2:17">
-      <c r="B12" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="37" t="s">
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="2"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="I16" s="15"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+    </row>
+    <row r="17" spans="1:38">
+      <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+    </row>
+    <row r="18" spans="1:38">
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+    </row>
+    <row r="19" spans="1:38">
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="20"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="2:17">
-      <c r="B13" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="37" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+    </row>
+    <row r="20" spans="1:38">
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="20"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="2:17">
-      <c r="B14" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="40" t="s">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+    </row>
+    <row r="22" spans="1:38">
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="20"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-    </row>
-    <row r="15" spans="2:17">
-      <c r="I15" s="23"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-    </row>
-    <row r="16" spans="2:17">
-      <c r="I16" s="21"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-    </row>
-    <row r="17" spans="1:38">
-      <c r="B17" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="20"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-    </row>
-    <row r="18" spans="1:38">
-      <c r="B18" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="20"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-    </row>
-    <row r="19" spans="1:38">
-      <c r="B19" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="37" t="s">
+    </row>
+    <row r="23" spans="1:38" ht="24">
+      <c r="B23" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" ht="24">
+      <c r="B24" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" ht="24">
+      <c r="B25" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:38">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:38">
+      <c r="A28" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="P28" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="R28" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF28" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL28" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" s="29" customFormat="1" ht="60">
+      <c r="A29" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="O29" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="P29" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q29" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="R29" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="S29" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="T29" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="U29" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="V29" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="W29" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="X29" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y29" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z29" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA29" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC29" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD29" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE29" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF29" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG29" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH29" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI29" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ29" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK29" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL29" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" s="31" customFormat="1">
+      <c r="A30" s="30">
+        <v>22</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="K30" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="L30" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="M30" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="N30" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O30" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="P30" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q30" s="31">
+        <v>12345</v>
+      </c>
+      <c r="R30" s="30">
+        <v>293</v>
+      </c>
+      <c r="S30" s="30">
+        <v>419</v>
+      </c>
+      <c r="T30" s="31">
+        <v>123</v>
+      </c>
+      <c r="U30" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="V30" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="W30" s="31">
+        <v>123456789</v>
+      </c>
+      <c r="X30" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y30" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-    </row>
-    <row r="20" spans="1:38">
-      <c r="B20" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="20"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-    </row>
-    <row r="22" spans="1:38">
-      <c r="B22" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="41" t="s">
+      <c r="Z30" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA30" s="30">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:38" ht="24">
-      <c r="B23" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:38" ht="24">
-      <c r="B24" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" ht="24">
-      <c r="B25" s="26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38">
-      <c r="B26" s="19"/>
-    </row>
-    <row r="27" spans="1:38">
-      <c r="B27" s="19"/>
-    </row>
-    <row r="28" spans="1:38">
-      <c r="A28" s="27" t="s">
+      <c r="AB30" s="30">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="AC30" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD30" s="30"/>
+      <c r="AE30" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF30" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG30" s="31">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI30" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ30" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL30" s="30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" s="31" customFormat="1">
+      <c r="B31" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="31">
+        <v>963357.1</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="L31" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="M31" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="N31" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O31" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="P31" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="30">
+        <v>293</v>
+      </c>
+      <c r="S31" s="30">
+        <v>419</v>
+      </c>
+      <c r="T31" s="33"/>
+      <c r="U31" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="V31" s="33"/>
+      <c r="W31" s="33"/>
+      <c r="X31" s="33"/>
+      <c r="Y31" s="33"/>
+      <c r="Z31" s="33"/>
+      <c r="AA31" s="30">
+        <v>97</v>
+      </c>
+      <c r="AB31" s="30">
         <v>8</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="P28" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="R28" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="U28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y28" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z28" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE28" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF28" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL28" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" s="29" customFormat="1" ht="60">
-      <c r="A29" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="K29" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="32" t="s">
+      <c r="AC31" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD31" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE31" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF31" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG31" s="31">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI31" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ31" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL31" s="30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" s="31" customFormat="1">
+      <c r="B32" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="31">
+        <v>963357.2</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="L32" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="M32" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="N32" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O32" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="P32" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="30">
+        <v>293</v>
+      </c>
+      <c r="S32" s="30">
+        <v>419</v>
+      </c>
+      <c r="T32" s="33"/>
+      <c r="U32" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="V32" s="33"/>
+      <c r="W32" s="33"/>
+      <c r="X32" s="33"/>
+      <c r="Y32" s="33"/>
+      <c r="Z32" s="33"/>
+      <c r="AA32" s="30">
+        <v>98</v>
+      </c>
+      <c r="AB32" s="30">
         <v>9</v>
       </c>
-      <c r="M29" s="32" t="s">
+      <c r="AC32" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD32" s="30"/>
+      <c r="AE32" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF32" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG32" s="31">
         <v>1</v>
       </c>
-      <c r="N29" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="O29" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q29" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="R29" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="S29" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="T29" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="U29" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="V29" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="W29" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="X29" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y29" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z29" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA29" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC29" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD29" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE29" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF29" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG29" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH29" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI29" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ29" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK29" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL29" s="35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" s="47" customFormat="1">
-      <c r="A30" s="45">
-        <v>22</v>
-      </c>
-      <c r="B30" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" s="46" t="s">
+      <c r="AH32" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI32" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ32" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK32" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL32" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:38" s="31" customFormat="1">
+      <c r="B33" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="31">
+        <v>963357.2</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="L33" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="M33" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="N33" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O33" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="P33" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="30">
+        <v>293</v>
+      </c>
+      <c r="S33" s="30">
+        <v>419</v>
+      </c>
+      <c r="T33" s="33"/>
+      <c r="U33" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="V33" s="33"/>
+      <c r="W33" s="33"/>
+      <c r="X33" s="33"/>
+      <c r="Y33" s="33"/>
+      <c r="Z33" s="33"/>
+      <c r="AA33" s="30">
+        <v>98</v>
+      </c>
+      <c r="AB33" s="30">
+        <v>9</v>
+      </c>
+      <c r="AC33" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD33" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE33" s="30"/>
+      <c r="AF33" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="46">
-        <v>963357</v>
-      </c>
-      <c r="E30" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G30" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="H30" s="47" t="s">
+      <c r="AG33" s="31">
+        <v>1</v>
+      </c>
+      <c r="AH33" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="I30" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="J30" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="K30" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="L30" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="M30" t="s">
-        <v>104</v>
-      </c>
-      <c r="N30" s="47" t="s">
+      <c r="AI33" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ33" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="O30" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="P30" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q30" s="47">
-        <v>12345</v>
-      </c>
-      <c r="R30" s="45">
-        <v>293</v>
-      </c>
-      <c r="S30" s="45">
-        <v>419</v>
-      </c>
-      <c r="T30" s="47">
+      <c r="AK33" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="U30" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="V30" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="W30" s="47">
-        <v>123456789</v>
-      </c>
-      <c r="X30" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y30" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z30" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA30" s="45">
-        <v>96</v>
-      </c>
-      <c r="AB30" s="45">
-        <v>7.4000000953674316</v>
-      </c>
-      <c r="AC30" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD30" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE30" s="45" t="s">
+      <c r="AL33" s="30" t="s">
         <v>73</v>
-      </c>
-      <c r="AF30" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG30" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH30" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI30" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ30" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK30" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL30" s="45" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" s="47" customFormat="1">
-      <c r="A31" s="7"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="L31" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="M31" t="s">
-        <v>108</v>
-      </c>
-      <c r="N31" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="O31" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="P31" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="45">
-        <v>293</v>
-      </c>
-      <c r="S31" s="45">
-        <v>419</v>
-      </c>
-      <c r="T31" s="22"/>
-      <c r="U31" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="V31" s="22"/>
-      <c r="W31" s="22"/>
-      <c r="X31" s="22"/>
-      <c r="Y31" s="22"/>
-      <c r="Z31" s="22"/>
-      <c r="AA31" s="45">
-        <v>97</v>
-      </c>
-      <c r="AB31" s="45">
-        <v>8</v>
-      </c>
-      <c r="AC31" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD31" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE31" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF31" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG31" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH31" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI31" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ31" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK31" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL31" s="45" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" s="47" customFormat="1">
-      <c r="A32" s="7"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="L32" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="M32" t="s">
-        <v>109</v>
-      </c>
-      <c r="N32" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="O32" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="P32" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="45">
-        <v>293</v>
-      </c>
-      <c r="S32" s="45">
-        <v>419</v>
-      </c>
-      <c r="T32" s="22"/>
-      <c r="U32" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="V32" s="22"/>
-      <c r="W32" s="22"/>
-      <c r="X32" s="22"/>
-      <c r="Y32" s="22"/>
-      <c r="Z32" s="22"/>
-      <c r="AA32" s="45">
-        <v>98</v>
-      </c>
-      <c r="AB32" s="45">
-        <v>9</v>
-      </c>
-      <c r="AC32" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD32" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE32" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF32" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG32" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH32" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI32" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ32" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK32" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL32" s="45" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPLIM-4712 make insert size be a range reported in the pipeline query.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
+    <workbookView xWindow="780" yWindow="560" windowWidth="31140" windowHeight="12260"/>
   </bookViews>
   <sheets>
     <sheet name="New Technology Lib Kit" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
   <si>
     <t>Total Library Volume (ul)</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -333,9 +333,6 @@
     <t>Lib-MOCK.FSK1.A</t>
   </si>
   <si>
-    <t>NovaSeq</t>
-  </si>
-  <si>
     <t>MOCK.FSK1.B</t>
   </si>
   <si>
@@ -400,13 +397,58 @@
   </si>
   <si>
     <t>Lib-MOCK.FSK1.A2</t>
+  </si>
+  <si>
+    <t>250-325</t>
+  </si>
+  <si>
+    <t>100-100</t>
+  </si>
+  <si>
+    <t>10.666</t>
+  </si>
+  <si>
+    <t>418</t>
+  </si>
+  <si>
+    <t>417</t>
+  </si>
+  <si>
+    <t>416</t>
+  </si>
+  <si>
+    <t>WholeGenomeShotgun.Resequencing</t>
+  </si>
+  <si>
+    <t>cDNAShotgunReadTwoSense.AssemblyWithoutReference</t>
+  </si>
+  <si>
+    <t>cDNAShotgunReadTwoSense.Resequencing</t>
+  </si>
+  <si>
+    <t>MiSeq</t>
+  </si>
+  <si>
+    <t>G96213</t>
+  </si>
+  <si>
+    <t>G96227</t>
+  </si>
+  <si>
+    <t>HiSeq X 10</t>
+  </si>
+  <si>
+    <t>NovaSeq S4</t>
+  </si>
+  <si>
+    <t>NextSeq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -645,6 +687,10 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Reference Sans Serif"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1014,7 +1060,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="182">
+  <cellStyleXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -1200,8 +1246,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1274,17 +1329,20 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="182">
+  <cellStyles count="191">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="120"/>
     <cellStyle name="20% - Accent2" xfId="93" builtinId="34" customBuiltin="1"/>
@@ -1434,6 +1492,15 @@
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="77" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="73" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="74" builtinId="17" customBuiltin="1"/>
@@ -1867,8 +1934,8 @@
   </sheetPr>
   <dimension ref="A2:AL33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1971,8 +2038,8 @@
       <c r="H5" s="7"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -1990,8 +2057,8 @@
       <c r="J6" s="10"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -2307,7 +2374,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:38" s="29" customFormat="1" ht="60">
+    <row r="29" spans="1:38" s="29" customFormat="1" ht="61" customHeight="1">
       <c r="A29" s="23" t="s">
         <v>3</v>
       </c>
@@ -2423,380 +2490,378 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:38" s="31" customFormat="1">
-      <c r="A30" s="30">
+    <row r="30" spans="1:38" s="32" customFormat="1" ht="13">
+      <c r="A30" s="31">
         <v>22</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="G30" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="K30" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="L30" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="N30" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="O30" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="P30" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q30" s="32">
+        <v>12345</v>
+      </c>
+      <c r="R30" s="31">
+        <v>293</v>
+      </c>
+      <c r="S30" s="31">
+        <v>419</v>
+      </c>
+      <c r="T30" s="32">
+        <v>123</v>
+      </c>
+      <c r="U30" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="V30" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="W30" s="32">
+        <v>123456789</v>
+      </c>
+      <c r="X30" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y30" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z30" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA30" s="31">
+        <v>96</v>
+      </c>
+      <c r="AB30" s="31">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="AC30" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD30" s="31"/>
+      <c r="AE30" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="AF30" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG30" s="32">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI30" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ30" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL30" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" s="32" customFormat="1" ht="13">
+      <c r="B31" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="32">
+        <v>963357.1</v>
+      </c>
+      <c r="E31" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="30" t="s">
+      <c r="F31" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="I30" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="K30" s="30" t="s">
+      <c r="L31" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="O31" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="P31" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q31" s="34"/>
+      <c r="R31" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="S31" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="T31" s="34"/>
+      <c r="U31" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
+      <c r="X31" s="34"/>
+      <c r="Y31" s="34"/>
+      <c r="Z31" s="34"/>
+      <c r="AA31" s="31">
+        <v>97</v>
+      </c>
+      <c r="AB31" s="31">
+        <v>8</v>
+      </c>
+      <c r="AC31" s="31"/>
+      <c r="AD31" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE31" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF31" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG31" s="32">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI31" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ31" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL31" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" s="32" customFormat="1" ht="13">
+      <c r="B32" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="32">
+        <v>963357.2</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="L30" s="30" t="s">
+      <c r="L32" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="M30" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="N30" s="31" t="s">
+      <c r="M32" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="N32" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="P30" s="31" t="s">
+      <c r="O32" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="P32" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="Q30" s="31">
-        <v>12345</v>
-      </c>
-      <c r="R30" s="30">
-        <v>293</v>
-      </c>
-      <c r="S30" s="30">
-        <v>419</v>
-      </c>
-      <c r="T30" s="31">
-        <v>123</v>
-      </c>
-      <c r="U30" s="30" t="s">
+      <c r="Q32" s="34"/>
+      <c r="R32" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="S32" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="T32" s="34"/>
+      <c r="U32" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="W30" s="31">
-        <v>123456789</v>
-      </c>
-      <c r="X30" s="31" t="s">
+      <c r="V32" s="34"/>
+      <c r="W32" s="34"/>
+      <c r="X32" s="34"/>
+      <c r="Y32" s="34"/>
+      <c r="Z32" s="34"/>
+      <c r="AA32" s="31">
         <v>98</v>
       </c>
-      <c r="Y30" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z30" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA30" s="30">
-        <v>96</v>
-      </c>
-      <c r="AB30" s="30">
-        <v>7.4000000953674316</v>
-      </c>
-      <c r="AC30" s="30" t="s">
+      <c r="AB32" s="31">
+        <v>9</v>
+      </c>
+      <c r="AC32" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="AD30" s="30"/>
-      <c r="AE30" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF30" s="32" t="s">
+      <c r="AD32" s="31"/>
+      <c r="AE32" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF32" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="AG30" s="31">
+      <c r="AG32" s="32">
         <v>1</v>
       </c>
-      <c r="AH30" s="31" t="s">
+      <c r="AH32" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="AI30" s="30" t="s">
+      <c r="AI32" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="AJ30" s="31" t="s">
+      <c r="AJ32" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="AL30" s="30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" s="31" customFormat="1">
-      <c r="B31" s="30" t="s">
+      <c r="AK32" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL32" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:38" s="32" customFormat="1" ht="13">
+      <c r="B33" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C33" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="31">
-        <v>963357.1</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="30" t="s">
+      <c r="D33" s="32">
+        <v>963357.2</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L31" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="M31" s="30" t="s">
+      <c r="L33" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="M33" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="N31" s="31" t="s">
+      <c r="N33" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="O31" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="P31" s="31" t="s">
+      <c r="O33" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="P33" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="30">
-        <v>293</v>
-      </c>
-      <c r="S31" s="30">
-        <v>419</v>
-      </c>
-      <c r="T31" s="33"/>
-      <c r="U31" s="30" t="s">
+      <c r="Q33" s="34"/>
+      <c r="R33" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="S33" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="T33" s="34"/>
+      <c r="U33" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="V31" s="33"/>
-      <c r="W31" s="33"/>
-      <c r="X31" s="33"/>
-      <c r="Y31" s="33"/>
-      <c r="Z31" s="33"/>
-      <c r="AA31" s="30">
-        <v>97</v>
-      </c>
-      <c r="AB31" s="30">
-        <v>8</v>
-      </c>
-      <c r="AC31" s="30" t="s">
+      <c r="V33" s="34"/>
+      <c r="W33" s="34"/>
+      <c r="X33" s="34"/>
+      <c r="Y33" s="34"/>
+      <c r="Z33" s="34"/>
+      <c r="AA33" s="31">
+        <v>98</v>
+      </c>
+      <c r="AB33" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC33" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="AD31" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE31" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF31" s="32" t="s">
+      <c r="AD33" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE33" s="31"/>
+      <c r="AF33" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="AG31" s="31">
+      <c r="AG33" s="32">
         <v>1</v>
       </c>
-      <c r="AH31" s="31" t="s">
+      <c r="AH33" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="AI31" s="30" t="s">
+      <c r="AI33" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="AJ31" s="31" t="s">
+      <c r="AJ33" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="AL31" s="30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" s="31" customFormat="1">
-      <c r="B32" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="31">
-        <v>963357.2</v>
-      </c>
-      <c r="E32" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="L32" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="M32" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="N32" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="O32" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="P32" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="30">
-        <v>293</v>
-      </c>
-      <c r="S32" s="30">
-        <v>419</v>
-      </c>
-      <c r="T32" s="33"/>
-      <c r="U32" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="V32" s="33"/>
-      <c r="W32" s="33"/>
-      <c r="X32" s="33"/>
-      <c r="Y32" s="33"/>
-      <c r="Z32" s="33"/>
-      <c r="AA32" s="30">
-        <v>98</v>
-      </c>
-      <c r="AB32" s="30">
-        <v>9</v>
-      </c>
-      <c r="AC32" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD32" s="30"/>
-      <c r="AE32" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF32" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG32" s="31">
-        <v>1</v>
-      </c>
-      <c r="AH32" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI32" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ32" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK32" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL32" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="2:38" s="31" customFormat="1">
-      <c r="B33" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="31">
-        <v>963357.2</v>
-      </c>
-      <c r="E33" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="L33" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="M33" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="N33" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="O33" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="P33" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="30">
-        <v>293</v>
-      </c>
-      <c r="S33" s="30">
-        <v>419</v>
-      </c>
-      <c r="T33" s="33"/>
-      <c r="U33" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="V33" s="33"/>
-      <c r="W33" s="33"/>
-      <c r="X33" s="33"/>
-      <c r="Y33" s="33"/>
-      <c r="Z33" s="33"/>
-      <c r="AA33" s="30">
-        <v>98</v>
-      </c>
-      <c r="AB33" s="30">
-        <v>9</v>
-      </c>
-      <c r="AC33" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD33" s="30" t="s">
+      <c r="AK33" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="AE33" s="30"/>
-      <c r="AF33" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG33" s="31">
-        <v>1</v>
-      </c>
-      <c r="AH33" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI33" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ33" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK33" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="AL33" s="30" t="s">
+      <c r="AL33" s="31" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GPLIM-4712 send sample kit request email
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="138">
   <si>
     <t>Total Library Volume (ul)</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -405,18 +405,12 @@
     <t>100-100</t>
   </si>
   <si>
-    <t>10.666</t>
-  </si>
-  <si>
     <t>418</t>
   </si>
   <si>
     <t>417</t>
   </si>
   <si>
-    <t>416</t>
-  </si>
-  <si>
     <t>WholeGenomeShotgun.Resequencing</t>
   </si>
   <si>
@@ -442,6 +436,9 @@
   </si>
   <si>
     <t>NextSeq</t>
+  </si>
+  <si>
+    <t>2137B</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1057,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -1205,6 +1202,8 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1329,9 +1328,6 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1341,8 +1337,11 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="193">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="120"/>
     <cellStyle name="20% - Accent2" xfId="93" builtinId="34" customBuiltin="1"/>
@@ -1501,6 +1500,8 @@
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="77" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="73" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="74" builtinId="17" customBuiltin="1"/>
@@ -1934,8 +1935,8 @@
   </sheetPr>
   <dimension ref="A2:AL33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="J9" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2038,8 +2039,8 @@
       <c r="H5" s="7"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -2057,8 +2058,8 @@
       <c r="J6" s="10"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -2086,7 +2087,9 @@
       <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -2490,378 +2493,376 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:38" s="32" customFormat="1" ht="13">
-      <c r="A30" s="31">
+    <row r="30" spans="1:38" s="31" customFormat="1" ht="13">
+      <c r="A30" s="30">
         <v>22</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="K30" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="L30" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="M30" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="N30" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O30" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="P30" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q30" s="31">
+        <v>12345</v>
+      </c>
+      <c r="R30" s="30">
+        <v>293</v>
+      </c>
+      <c r="S30" s="30">
+        <v>419</v>
+      </c>
+      <c r="T30" s="31">
+        <v>123</v>
+      </c>
+      <c r="U30" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="V30" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="W30" s="31">
+        <v>123456789</v>
+      </c>
+      <c r="X30" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y30" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z30" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA30" s="30">
+        <v>96</v>
+      </c>
+      <c r="AB30" s="30">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="AC30" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD30" s="30"/>
+      <c r="AE30" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF30" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG30" s="31">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI30" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ30" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL30" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" s="31" customFormat="1" ht="13">
+      <c r="B31" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="31">
+        <v>963357.1</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="L31" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="M31" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="N31" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="O31" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="P31" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="S31" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="T31" s="33"/>
+      <c r="U31" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="V31" s="33"/>
+      <c r="W31" s="33"/>
+      <c r="X31" s="33"/>
+      <c r="Y31" s="33"/>
+      <c r="Z31" s="33"/>
+      <c r="AA31" s="30">
+        <v>97</v>
+      </c>
+      <c r="AB31" s="30">
+        <v>8</v>
+      </c>
+      <c r="AC31" s="30"/>
+      <c r="AD31" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE31" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF31" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG31" s="31">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI31" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ31" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL31" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" s="31" customFormat="1" ht="13">
+      <c r="B32" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="31">
+        <v>963357.2</v>
+      </c>
+      <c r="E32" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G30" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="I30" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="J30" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="K30" s="31" t="s">
+      <c r="F32" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="L30" s="31" t="s">
+      <c r="L32" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="M30" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="N30" s="32" t="s">
+      <c r="M32" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="N32" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="P30" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q30" s="32">
-        <v>12345</v>
-      </c>
-      <c r="R30" s="31">
-        <v>293</v>
-      </c>
-      <c r="S30" s="31">
-        <v>419</v>
-      </c>
-      <c r="T30" s="32">
-        <v>123</v>
-      </c>
-      <c r="U30" s="31" t="s">
+      <c r="O32" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="P32" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="S32" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="T32" s="33"/>
+      <c r="U32" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="W30" s="32">
-        <v>123456789</v>
-      </c>
-      <c r="X30" s="32" t="s">
+      <c r="V32" s="33"/>
+      <c r="W32" s="33"/>
+      <c r="X32" s="33"/>
+      <c r="Y32" s="33"/>
+      <c r="Z32" s="33"/>
+      <c r="AA32" s="30">
         <v>98</v>
       </c>
-      <c r="Y30" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z30" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA30" s="31">
-        <v>96</v>
-      </c>
-      <c r="AB30" s="31">
-        <v>7.4000000953674316</v>
-      </c>
-      <c r="AC30" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD30" s="31"/>
-      <c r="AE30" s="31" t="s">
+      <c r="AB32" s="30">
+        <v>9</v>
+      </c>
+      <c r="AC32" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD32" s="30"/>
+      <c r="AE32" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="AF30" s="33" t="s">
+      <c r="AF32" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="AG30" s="32">
+      <c r="AG32" s="31">
         <v>1</v>
       </c>
-      <c r="AH30" s="32" t="s">
+      <c r="AH32" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="AI30" s="31" t="s">
+      <c r="AI32" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="AJ30" s="32" t="s">
+      <c r="AJ32" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="AL30" s="31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" s="32" customFormat="1" ht="13">
-      <c r="B31" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="32">
-        <v>963357.1</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="31" t="s">
+      <c r="AK32" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL32" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:38" s="31" customFormat="1" ht="13">
+      <c r="B33" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="31">
+        <v>963357.2</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="L31" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="M31" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="N31" s="32" t="s">
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="L33" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="M33" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="N33" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="O31" s="32" t="s">
+      <c r="O33" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="P31" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q31" s="34"/>
-      <c r="R31" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="S31" s="31" t="s">
+      <c r="P33" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="S33" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="T31" s="34"/>
-      <c r="U31" s="31" t="s">
+      <c r="T33" s="33"/>
+      <c r="U33" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="V31" s="34"/>
-      <c r="W31" s="34"/>
-      <c r="X31" s="34"/>
-      <c r="Y31" s="34"/>
-      <c r="Z31" s="34"/>
-      <c r="AA31" s="31">
-        <v>97</v>
-      </c>
-      <c r="AB31" s="31">
-        <v>8</v>
-      </c>
-      <c r="AC31" s="31"/>
-      <c r="AD31" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE31" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF31" s="33" t="s">
+      <c r="V33" s="33"/>
+      <c r="W33" s="33"/>
+      <c r="X33" s="33"/>
+      <c r="Y33" s="33"/>
+      <c r="Z33" s="33"/>
+      <c r="AA33" s="30">
+        <v>98</v>
+      </c>
+      <c r="AB33" s="30"/>
+      <c r="AC33" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD33" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE33" s="30"/>
+      <c r="AF33" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="AG31" s="32">
+      <c r="AG33" s="31">
         <v>1</v>
       </c>
-      <c r="AH31" s="32" t="s">
+      <c r="AH33" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="AI31" s="31" t="s">
+      <c r="AI33" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="AJ31" s="32" t="s">
+      <c r="AJ33" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="AL31" s="31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" s="32" customFormat="1" ht="13">
-      <c r="B32" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="32">
-        <v>963357.2</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="L32" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="M32" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="N32" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="O32" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="P32" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="S32" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="T32" s="34"/>
-      <c r="U32" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="V32" s="34"/>
-      <c r="W32" s="34"/>
-      <c r="X32" s="34"/>
-      <c r="Y32" s="34"/>
-      <c r="Z32" s="34"/>
-      <c r="AA32" s="31">
-        <v>98</v>
-      </c>
-      <c r="AB32" s="31">
-        <v>9</v>
-      </c>
-      <c r="AC32" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD32" s="31"/>
-      <c r="AE32" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF32" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG32" s="32">
-        <v>1</v>
-      </c>
-      <c r="AH32" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI32" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ32" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK32" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL32" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="2:38" s="32" customFormat="1" ht="13">
-      <c r="B33" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="32">
-        <v>963357.2</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="L33" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="M33" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="N33" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="O33" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="P33" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="S33" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="T33" s="34"/>
-      <c r="U33" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="V33" s="34"/>
-      <c r="W33" s="34"/>
-      <c r="X33" s="34"/>
-      <c r="Y33" s="34"/>
-      <c r="Z33" s="34"/>
-      <c r="AA33" s="31">
-        <v>98</v>
-      </c>
-      <c r="AB33" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC33" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD33" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="AE33" s="31"/>
-      <c r="AF33" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG33" s="32">
-        <v>1</v>
-      </c>
-      <c r="AH33" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI33" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ33" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK33" s="32" t="s">
+      <c r="AK33" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="AL33" s="31" t="s">
+      <c r="AL33" s="30" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GPLIM-4712 add changes from discussion with users including new columns in Pooled Tube spreadsheet
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryEZPassTest.xlsx
@@ -10,7 +10,7 @@
     <sheet name="New Technology Lib Kit" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'New Technology Lib Kit'!$A$1:$AK$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'New Technology Lib Kit'!$A$1:$AK$23</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="127">
   <si>
     <t>Total Library Volume (ul)</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -50,9 +50,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>*Note Columns in Red are Mandatory for all Samples and Columns in Green are Mandatory for EZPASS samples</t>
-  </si>
-  <si>
     <t>Individual Name (aka Patient ID, Required for human subject samples)</t>
   </si>
   <si>
@@ -90,18 +87,6 @@
   </si>
   <si>
     <t>Source Sample GSSR ID</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>Mandatory for all samples</t>
-  </si>
-  <si>
-    <t>Mandatory for EZPASS samples</t>
-  </si>
-  <si>
-    <t>Mandatory for Kiosk samples</t>
   </si>
   <si>
     <t>Additional Sample Information</t>
@@ -201,36 +186,6 @@
     <t>Molecular Barcode Sequence</t>
   </si>
   <si>
-    <t>Don't need this stuff</t>
-  </si>
-  <si>
-    <t>Can write anything here</t>
-  </si>
-  <si>
-    <t>mean or peak is best</t>
-  </si>
-  <si>
-    <t>Keep Blank</t>
-  </si>
-  <si>
-    <t>Collaborator, ticket no.</t>
-  </si>
-  <si>
-    <t>do not need path</t>
-  </si>
-  <si>
-    <t>look up in tableau</t>
-  </si>
-  <si>
-    <t>Column O (Collaborator Sample ID)</t>
-  </si>
-  <si>
-    <t>Column M (Collaborator Participant ID)</t>
-  </si>
-  <si>
-    <t>SM-(Column A)  but for this set (Column B) (Sample ID)</t>
-  </si>
-  <si>
     <t>Virtual GSSR ID</t>
   </si>
   <si>
@@ -306,9 +261,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>AAGGCTAT</t>
   </si>
   <si>
@@ -439,13 +391,28 @@
   </si>
   <si>
     <t>2137B</t>
+  </si>
+  <si>
+    <t>Cell color indicates:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Required </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Required Once per Tube </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Optional </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ignored </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -526,13 +493,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
@@ -729,12 +689,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
@@ -908,12 +862,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor indexed="14"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1056,6 +1016,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1132,75 +1129,75 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1255,7 +1252,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1292,21 +1289,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1316,7 +1298,7 @@
     <xf numFmtId="49" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1328,18 +1310,23 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="193">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
@@ -1933,10 +1920,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AL33"/>
+  <dimension ref="A2:AL27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J9" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30:F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1982,10 +1969,12 @@
   <sheetData>
     <row r="2" spans="2:17">
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="29" t="s">
+        <v>122</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="M2" s="4"/>
@@ -1996,10 +1985,12 @@
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="30" t="s">
+        <v>123</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="M3" s="12"/>
@@ -2010,12 +2001,14 @@
     </row>
     <row r="4" spans="2:17">
       <c r="B4" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="9"/>
+        <v>67</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>124</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="J4" s="10"/>
@@ -2029,47 +2022,51 @@
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>68</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>125</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="2:17">
       <c r="B6" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>126</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="J6" s="10"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="2:17">
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2085,10 +2082,10 @@
     </row>
     <row r="8" spans="2:17">
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -2103,10 +2100,10 @@
     </row>
     <row r="9" spans="2:17">
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2121,10 +2118,10 @@
     </row>
     <row r="10" spans="2:17">
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2139,7 +2136,7 @@
     </row>
     <row r="11" spans="2:17">
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2">
         <v>2215</v>
@@ -2157,10 +2154,10 @@
     </row>
     <row r="12" spans="2:17">
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2175,10 +2172,10 @@
     </row>
     <row r="13" spans="2:17">
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -2193,10 +2190,10 @@
     </row>
     <row r="14" spans="2:17">
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -2228,7 +2225,7 @@
     </row>
     <row r="17" spans="1:38">
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C17" s="2"/>
       <c r="F17" s="2"/>
@@ -2243,7 +2240,7 @@
     </row>
     <row r="18" spans="1:38">
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C18" s="2"/>
       <c r="F18" s="2"/>
@@ -2258,10 +2255,10 @@
     </row>
     <row r="19" spans="1:38">
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2274,10 +2271,10 @@
     </row>
     <row r="20" spans="1:38">
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -2290,580 +2287,495 @@
       <c r="P20" s="11"/>
     </row>
     <row r="22" spans="1:38">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:38" s="22" customFormat="1" ht="61" customHeight="1">
+      <c r="A23" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="H23" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="P23" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q23" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="R23" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S23" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="T23" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="U23" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="V23" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="W23" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="X23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y23" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z23" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA23" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC23" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD23" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE23" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF23" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG23" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH23" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI23" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ23" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK23" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL23" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" s="24" customFormat="1" ht="13">
+      <c r="A24" s="23">
+        <v>22</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="N24" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="O24" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="P24" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q24" s="24">
+        <v>12345</v>
+      </c>
+      <c r="R24" s="23">
+        <v>293</v>
+      </c>
+      <c r="S24" s="23">
+        <v>419</v>
+      </c>
+      <c r="T24" s="24">
+        <v>123</v>
+      </c>
+      <c r="U24" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="V24" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="W24" s="24">
+        <v>123456789</v>
+      </c>
+      <c r="X24" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y24" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z24" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA24" s="23">
+        <v>96</v>
+      </c>
+      <c r="AB24" s="23">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="AC24" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD24" s="23"/>
+      <c r="AE24" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF24" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG24" s="24">
+        <v>1</v>
+      </c>
+      <c r="AH24" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI24" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ24" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL24" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" s="24" customFormat="1" ht="13">
+      <c r="B25" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="C25" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="24">
+        <v>963357.1</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="L25" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="M25" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="N25" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="O25" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="P25" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="S25" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="T25" s="26"/>
+      <c r="U25" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="V25" s="26"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="26"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="23">
+        <v>97</v>
+      </c>
+      <c r="AB25" s="23">
+        <v>8</v>
+      </c>
+      <c r="AC25" s="23"/>
+      <c r="AD25" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE25" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF25" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG25" s="24">
+        <v>1</v>
+      </c>
+      <c r="AH25" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI25" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ25" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL25" s="23" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="23" spans="1:38" ht="24">
-      <c r="B23" s="16" t="s">
-        <v>23</v>
+    <row r="26" spans="1:38" s="24" customFormat="1" ht="13">
+      <c r="B26" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="24">
+        <v>963357.2</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="L26" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="N26" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="O26" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="S26" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="T26" s="26"/>
+      <c r="U26" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="23">
+        <v>98</v>
+      </c>
+      <c r="AB26" s="23">
+        <v>9</v>
+      </c>
+      <c r="AC26" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD26" s="23"/>
+      <c r="AE26" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF26" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG26" s="24">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI26" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ26" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK26" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL26" s="23" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="24">
-      <c r="B24" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" ht="24">
-      <c r="B25" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38">
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:38">
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:38">
-      <c r="A28" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="3" t="s">
+    <row r="27" spans="1:38" s="24" customFormat="1" ht="13">
+      <c r="B27" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="24">
+        <v>963357.2</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="L27" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="M27" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="N27" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="O27" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="P27" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="S27" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="T27" s="26"/>
+      <c r="U27" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="V27" s="26"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+      <c r="Y27" s="26"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="23">
+        <v>98</v>
+      </c>
+      <c r="AB27" s="23"/>
+      <c r="AC27" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD27" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE27" s="23"/>
+      <c r="AF27" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG27" s="24">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ27" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK27" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL27" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="P28" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="R28" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="U28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF28" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL28" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" s="29" customFormat="1" ht="61" customHeight="1">
-      <c r="A29" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="K29" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="M29" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="N29" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="O29" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q29" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="R29" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="S29" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="T29" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="U29" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="V29" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="W29" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="X29" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y29" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z29" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA29" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC29" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD29" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE29" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF29" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG29" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH29" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI29" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ29" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK29" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL29" s="28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" s="31" customFormat="1" ht="13">
-      <c r="A30" s="30">
-        <v>22</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="G30" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="I30" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="K30" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="L30" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="M30" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="N30" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="O30" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="P30" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q30" s="31">
-        <v>12345</v>
-      </c>
-      <c r="R30" s="30">
-        <v>293</v>
-      </c>
-      <c r="S30" s="30">
-        <v>419</v>
-      </c>
-      <c r="T30" s="31">
-        <v>123</v>
-      </c>
-      <c r="U30" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="V30" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="W30" s="31">
-        <v>123456789</v>
-      </c>
-      <c r="X30" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y30" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z30" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA30" s="30">
-        <v>96</v>
-      </c>
-      <c r="AB30" s="30">
-        <v>7.4000000953674316</v>
-      </c>
-      <c r="AC30" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD30" s="30"/>
-      <c r="AE30" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF30" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG30" s="31">
-        <v>1</v>
-      </c>
-      <c r="AH30" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI30" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ30" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL30" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" s="31" customFormat="1" ht="13">
-      <c r="B31" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="31">
-        <v>963357.1</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="L31" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="M31" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="N31" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="O31" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="P31" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="S31" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="T31" s="33"/>
-      <c r="U31" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="V31" s="33"/>
-      <c r="W31" s="33"/>
-      <c r="X31" s="33"/>
-      <c r="Y31" s="33"/>
-      <c r="Z31" s="33"/>
-      <c r="AA31" s="30">
-        <v>97</v>
-      </c>
-      <c r="AB31" s="30">
-        <v>8</v>
-      </c>
-      <c r="AC31" s="30"/>
-      <c r="AD31" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE31" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF31" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG31" s="31">
-        <v>1</v>
-      </c>
-      <c r="AH31" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI31" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ31" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL31" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" s="31" customFormat="1" ht="13">
-      <c r="B32" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="31">
-        <v>963357.2</v>
-      </c>
-      <c r="E32" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="L32" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="M32" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="N32" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="O32" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="P32" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="S32" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="T32" s="33"/>
-      <c r="U32" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="V32" s="33"/>
-      <c r="W32" s="33"/>
-      <c r="X32" s="33"/>
-      <c r="Y32" s="33"/>
-      <c r="Z32" s="33"/>
-      <c r="AA32" s="30">
-        <v>98</v>
-      </c>
-      <c r="AB32" s="30">
-        <v>9</v>
-      </c>
-      <c r="AC32" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD32" s="30"/>
-      <c r="AE32" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF32" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG32" s="31">
-        <v>1</v>
-      </c>
-      <c r="AH32" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI32" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ32" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK32" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL32" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="2:38" s="31" customFormat="1" ht="13">
-      <c r="B33" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="31">
-        <v>963357.2</v>
-      </c>
-      <c r="E33" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="L33" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="M33" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="N33" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="O33" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="P33" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="S33" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="T33" s="33"/>
-      <c r="U33" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="V33" s="33"/>
-      <c r="W33" s="33"/>
-      <c r="X33" s="33"/>
-      <c r="Y33" s="33"/>
-      <c r="Z33" s="33"/>
-      <c r="AA33" s="30">
-        <v>98</v>
-      </c>
-      <c r="AB33" s="30"/>
-      <c r="AC33" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD33" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="AE33" s="30"/>
-      <c r="AF33" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG33" s="31">
-        <v>1</v>
-      </c>
-      <c r="AH33" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI33" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ33" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK33" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="AL33" s="30" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>